<commit_message>
cambios codigo con bbdd 1000, 5000 etc.
</commit_message>
<xml_diff>
--- a/DatosPasos.xlsx
+++ b/DatosPasos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e32b480a36d69a14/Documents/Estudios/TFM/Codigo limpio Repo/TFM_Bagging_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{BE5219BF-41A0-4068-902D-52E74314BB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C13A3F51-F28C-4893-B390-380F5CFE2686}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{BE5219BF-41A0-4068-902D-52E74314BB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3928F564-8E2B-498F-B8DE-45844D4EE5F6}"/>
   <bookViews>
-    <workbookView xWindow="21570" yWindow="30" windowWidth="36030" windowHeight="23670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="30" windowWidth="36030" windowHeight="23670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +137,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -158,6 +164,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +471,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +645,24 @@
       <c r="D6" s="1">
         <v>0.75516693163751991</v>
       </c>
+      <c r="E6" s="2">
+        <v>0.732704402515723</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.74764890282131602</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.73241590214067198</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.75454545454545396</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.74422187981510002</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.73015873015873001</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -885,6 +911,24 @@
       <c r="D16" s="1">
         <v>0.90240770465489561</v>
       </c>
+      <c r="E16" s="2">
+        <v>0.88778454632895099</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.86408383613845596</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.84099673687333099</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.86887694145758598</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.87992884672398397</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.843621399176954</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -956,6 +1000,27 @@
       <c r="C20" s="1">
         <v>0.99690976514215079</v>
       </c>
+      <c r="D20" s="1">
+        <v>0.99664958612534493</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.99665222528554553</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.99741909866984313</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.99574310568202851</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.99576505247652369</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.99724416681976846</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.99666927899686519</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -965,6 +1030,27 @@
       <c r="C21" s="1">
         <v>0.99320148331273173</v>
       </c>
+      <c r="D21" s="1">
+        <v>0.99349625541978714</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.99487987396612843</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.99523525908278743</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.99481769387377383</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.99318725833179888</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.9950395002755833</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.99314263322884011</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -974,6 +1060,27 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
+      <c r="D22" s="1">
+        <v>0.99842333464722111</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.99881843245372193</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.99880881477069683</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.99925967055339626</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.9974222058552753</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.99816277787984564</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.99784482758620685</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -983,6 +1090,27 @@
       <c r="C23" s="1">
         <v>1</v>
       </c>
+      <c r="D23" s="1">
+        <v>0.99842333464722111</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.99862150452934229</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.9986102838991463</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.99925967055339626</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.99815871846805382</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.99853022230387656</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.99804075235109713</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -992,6 +1120,23 @@
       <c r="C24" s="1">
         <v>0.99505562422744132</v>
       </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="1">
+        <v>0.99703791469194314</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.99633296662999637</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.99628597957288767</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.99446085672082718</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.9941268598277212</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1001,6 +1146,27 @@
       <c r="C25" s="1">
         <v>0.99876390599999998</v>
       </c>
+      <c r="D25" s="1">
+        <v>0.99763500197083166</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.99763686490744385</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.99779735682819304</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.99907544378698199</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.99763500197083166</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.99763686490744385</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.99763500197083166</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1009,6 +1175,27 @@
       </c>
       <c r="C26" s="1">
         <v>0.99320148331273173</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.99290500591249509</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.99133517132729421</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.99384554298193373</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.99389228206551916</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.99208248941263122</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.99118133382325924</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.99275078369905956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>